<commit_message>
Add backup files, utility scripts, and framework updates
- Added backup files for ad-dashboard and pivot-table
- Added utility scripts for checking images and downloading missing ones
- Added Python scripts for extracting traits from framework
- Added CSV files tracking ads with broken/missing links
- Updated creative traits framework Excel file

🤖 Generated with [Claude Code](https://claude.com/claude-code)

Co-Authored-By: Claude <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/creative_traits_framework_full.xlsx
+++ b/creative_traits_framework_full.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/caiopimenta/Claude/top-ads-scorecard/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC1D5D10-186A-AB4B-BE15-3C31B320A035}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D887247-D6A0-3742-A9B2-0945B73987FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="20040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-38400" yWindow="1560" windowWidth="38400" windowHeight="20040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Creative Traits" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="78">
   <si>
     <t>Headline (Hook Text)</t>
   </si>
@@ -157,22 +157,10 @@
     <t>High Bills</t>
   </si>
   <si>
-    <t>Neutral</t>
-  </si>
-  <si>
     <t>Cool</t>
   </si>
   <si>
-    <t>Hard to Open</t>
-  </si>
-  <si>
     <t>Easy Operation</t>
-  </si>
-  <si>
-    <t>Outdated Look/Style</t>
-  </si>
-  <si>
-    <t>Modern Look</t>
   </si>
   <si>
     <t>Mold/Mildew</t>
@@ -208,9 +196,6 @@
     <t>Temperature Control</t>
   </si>
   <si>
-    <t>Drafty/Old/Leaky/Broken</t>
-  </si>
-  <si>
     <t>Energy Efficiency</t>
   </si>
   <si>
@@ -227,9 +212,6 @@
   </si>
   <si>
     <t>Human presence</t>
-  </si>
-  <si>
-    <t>Cost</t>
   </si>
   <si>
     <t>Y</t>
@@ -263,6 +245,15 @@
   </si>
   <si>
     <t>Hands Only</t>
+  </si>
+  <si>
+    <t>Outdated</t>
+  </si>
+  <si>
+    <t>BOGO / BNPL / $0 Down / Financing</t>
+  </si>
+  <si>
+    <t>Cost/Price</t>
   </si>
 </sst>
 </file>
@@ -651,7 +642,7 @@
   <dimension ref="A1:R1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M14" sqref="M14"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -701,22 +692,22 @@
         <v>40</v>
       </c>
       <c r="M1" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="N1" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="O1" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="P1" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="Q1" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="N1" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="O1" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="P1" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="Q1" s="5" t="s">
-        <v>74</v>
-      </c>
       <c r="R1" s="5" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.2">
@@ -724,10 +715,10 @@
         <v>10</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>62</v>
+        <v>44</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>41</v>
@@ -760,28 +751,28 @@
         <v>28</v>
       </c>
       <c r="N2" s="4" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="O2" s="4" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="P2" s="4" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="Q2" s="4" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="R2" s="4" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A3" s="4"/>
       <c r="B3" s="3" t="s">
-        <v>44</v>
+        <v>60</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>33</v>
@@ -809,31 +800,31 @@
         <v>45</v>
       </c>
       <c r="M3" s="3" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="N3" s="4" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="O3" s="4" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="P3" s="4" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="Q3" s="4" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="R3" s="4" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A4" s="4"/>
       <c r="B4" s="3" t="s">
-        <v>65</v>
+        <v>75</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>39</v>
@@ -857,11 +848,8 @@
       <c r="K4" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="L4" s="3" t="s">
-        <v>46</v>
-      </c>
       <c r="M4" s="4" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="N4" s="4"/>
       <c r="O4" s="4"/>
@@ -875,10 +863,10 @@
         <v>47</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>28</v>
+        <v>76</v>
       </c>
       <c r="E5" s="4"/>
       <c r="F5" s="3" t="s">
@@ -897,7 +885,7 @@
       <c r="K5" s="4"/>
       <c r="L5" s="4"/>
       <c r="M5" s="3" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="N5" s="4"/>
       <c r="O5" s="4"/>
@@ -911,9 +899,11 @@
         <v>49</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
-      <c r="D6" s="4"/>
+      <c r="D6" s="3" t="s">
+        <v>28</v>
+      </c>
       <c r="E6" s="4"/>
       <c r="F6" s="3" t="s">
         <v>29</v>
@@ -929,7 +919,7 @@
       <c r="K6" s="4"/>
       <c r="L6" s="4"/>
       <c r="M6" s="6" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="N6" s="4"/>
       <c r="O6" s="4"/>
@@ -940,10 +930,10 @@
     <row r="7" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A7" s="4"/>
       <c r="B7" s="3" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D7" s="4"/>
       <c r="E7" s="4"/>
@@ -968,17 +958,17 @@
     <row r="8" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A8" s="4"/>
       <c r="B8" s="3" t="s">
-        <v>53</v>
+        <v>77</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D8" s="4"/>
       <c r="E8" s="4"/>
       <c r="F8" s="4"/>
       <c r="G8" s="4"/>
       <c r="H8" s="3" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="I8" s="4"/>
       <c r="J8" s="4"/>
@@ -994,10 +984,10 @@
     <row r="9" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A9" s="4"/>
       <c r="B9" s="3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>57</v>
+        <v>32</v>
       </c>
       <c r="D9" s="4"/>
       <c r="E9" s="4"/>
@@ -1018,10 +1008,10 @@
     <row r="10" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A10" s="4"/>
       <c r="B10" s="3" t="s">
-        <v>69</v>
+        <v>32</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>32</v>
+        <v>55</v>
       </c>
       <c r="D10" s="4"/>
       <c r="E10" s="4"/>
@@ -1041,11 +1031,8 @@
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A11" s="4"/>
-      <c r="B11" s="3" t="s">
-        <v>58</v>
-      </c>
       <c r="C11" s="3" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D11" s="4"/>
       <c r="E11" s="4"/>
@@ -1065,11 +1052,8 @@
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A12" s="4"/>
-      <c r="B12" s="3" t="s">
-        <v>32</v>
-      </c>
       <c r="C12" s="3" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="D12" s="4"/>
       <c r="E12" s="4"/>
@@ -1091,7 +1075,7 @@
       <c r="A13" s="4"/>
       <c r="B13" s="4"/>
       <c r="C13" s="3" t="s">
-        <v>67</v>
+        <v>57</v>
       </c>
       <c r="D13" s="4"/>
       <c r="E13" s="4"/>
@@ -1112,9 +1096,6 @@
     <row r="14" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A14" s="4"/>
       <c r="B14" s="4"/>
-      <c r="C14" s="3" t="s">
-        <v>61</v>
-      </c>
       <c r="D14" s="4"/>
       <c r="E14" s="4"/>
       <c r="F14" s="4"/>

</xml_diff>